<commit_message>
On continue le datapath
</commit_message>
<xml_diff>
--- a/Tableaux_FRAM_DESE2em.xlsx
+++ b/Tableaux_FRAM_DESE2em.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03740260-BC31-4E2C-857A-A94C28BF6016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC1BF7F-985F-4CF0-ABA6-35E9AF0C6688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="0" windowWidth="17280" windowHeight="10665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="10665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau 1" sheetId="2" r:id="rId1"/>
@@ -1155,8 +1155,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>